<commit_message>
Clean up data files
</commit_message>
<xml_diff>
--- a/README.xlsx
+++ b/README.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pamelagreen/Desktop/Data/Griffith2022/scripts_swb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0987BF32-C8FB-8146-962B-BA3BFB0E2253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C99C7C4-1F12-5442-9350-C3FF6E0EC563}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43920" yWindow="1360" windowWidth="30840" windowHeight="16680" xr2:uid="{AC79CE72-321E-844F-A989-0FF187B9C603}"/>
+    <workbookView xWindow="41400" yWindow="-160" windowWidth="30840" windowHeight="16680" activeTab="1" xr2:uid="{AC79CE72-321E-844F-A989-0FF187B9C603}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="143">
   <si>
     <r>
       <rPr>
@@ -358,30 +358,6 @@
     <t>Local population from GPW4</t>
   </si>
   <si>
-    <t>WBM_TerraClimate2000-2020_Q_DIST_CV_InterAnnual_6min.tif</t>
-  </si>
-  <si>
-    <t>WBM_TerraClimate2000-2020_Q_DIST_CV_IntraAnnual_6min.tif</t>
-  </si>
-  <si>
-    <t>WBM_TerraClimate2000-2020_Q_DIST_meanCV_IntraAnnual_6min.tif</t>
-  </si>
-  <si>
-    <t>CV-CDF</t>
-  </si>
-  <si>
-    <t>unitless</t>
-  </si>
-  <si>
-    <t>Coefficient of Variation of monthly discharges over full time period 2000-2020</t>
-  </si>
-  <si>
-    <t>Coefficient of Variation of annual discharges over  time period 2000-2020</t>
-  </si>
-  <si>
-    <t>Coefficient of Variation of monthly discharges for mean annual discharge from 2000-2020</t>
-  </si>
-  <si>
     <t>Groundwater</t>
   </si>
   <si>
@@ -581,6 +557,36 @@
   </si>
   <si>
     <t>Data files belonging to manuscript: "How can we live within the safe and just Earth system boundaries for blue water?"</t>
+  </si>
+  <si>
+    <t>ESTRESS</t>
+  </si>
+  <si>
+    <t>PointSample_ESTRESS_Chg20.xlsx</t>
+  </si>
+  <si>
+    <t>Table of sub-basins with ESTRESS variables</t>
+  </si>
+  <si>
+    <t>Environmental Stress Aggregates for Sub-basins (Figure S1-a)</t>
+  </si>
+  <si>
+    <t>HydroSTN30_Subbasin_ESTRESS_Chg20.shp</t>
+  </si>
+  <si>
+    <t>Subbasin Shapefile file - IDs PointSample_ESTRESS_Chg20.xlsx</t>
+  </si>
+  <si>
+    <t>RGIS subbasins</t>
+  </si>
+  <si>
+    <t>Coast_2.shp</t>
+  </si>
+  <si>
+    <t>Global coast outline</t>
+  </si>
+  <si>
+    <t>Vector Coast outline</t>
   </si>
 </sst>
 </file>
@@ -989,7 +995,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7BDF3D2-F8D8-2E4A-8090-DA540BF4D3A7}">
   <dimension ref="A1:A14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="133" zoomScaleNormal="133" workbookViewId="0"/>
+    <sheetView zoomScale="133" zoomScaleNormal="133" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1003,7 +1009,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
@@ -1065,8 +1071,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0458106B-385E-2D4D-BF8D-F8C090212C36}">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1074,7 +1080,7 @@
     <col min="1" max="1" width="17.33203125" customWidth="1"/>
     <col min="2" max="2" width="61.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="46.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="53.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="61.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1095,130 +1101,130 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>69</v>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>133</v>
       </c>
       <c r="B3" t="s">
-        <v>66</v>
+        <v>134</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="D3" t="s">
-        <v>70</v>
+        <v>135</v>
       </c>
       <c r="E3" t="s">
-        <v>72</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>67</v>
+        <v>137</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="D4" t="s">
-        <v>70</v>
+        <v>138</v>
       </c>
       <c r="E4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" t="s">
         <v>68</v>
       </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" t="s">
-        <v>70</v>
-      </c>
-      <c r="E5" t="s">
-        <v>71</v>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
-        <v>74</v>
-      </c>
       <c r="B7" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="E7" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="E8" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C9" t="s">
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="E9" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C10" t="s">
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="E10" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
-        <v>80</v>
-      </c>
-      <c r="C11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" t="s">
-        <v>47</v>
-      </c>
-      <c r="E11" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>57</v>
       </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C13" t="s">
         <v>9</v>
@@ -1227,57 +1233,58 @@
         <v>26</v>
       </c>
       <c r="E13" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="C14" t="s">
         <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="E14" t="s">
-        <v>35</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>58</v>
+        <v>17</v>
       </c>
       <c r="C15" t="s">
         <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E15" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" t="s">
-        <v>60</v>
-      </c>
-      <c r="E16" t="s">
         <v>46</v>
       </c>
     </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" t="s">
+        <v>45</v>
+      </c>
+    </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="7" t="s">
-        <v>75</v>
-      </c>
+      <c r="A18" s="7"/>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C18" t="s">
         <v>9</v>
@@ -1286,13 +1293,13 @@
         <v>33</v>
       </c>
       <c r="E18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="7"/>
       <c r="B19" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C19" t="s">
         <v>9</v>
@@ -1301,13 +1308,12 @@
         <v>33</v>
       </c>
       <c r="E19" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="7"/>
       <c r="B20" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C20" t="s">
         <v>9</v>
@@ -1316,112 +1322,112 @@
         <v>33</v>
       </c>
       <c r="E20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B21" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" t="s">
-        <v>9</v>
-      </c>
-      <c r="D21" t="s">
-        <v>33</v>
-      </c>
-      <c r="E21" t="s">
         <v>43</v>
       </c>
     </row>
+    <row r="22" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" t="s">
+        <v>64</v>
+      </c>
+      <c r="E22" t="s">
+        <v>65</v>
+      </c>
+    </row>
     <row r="23" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>10</v>
-      </c>
+      <c r="A23" s="4"/>
       <c r="B23" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C23" t="s">
         <v>9</v>
       </c>
       <c r="D23" t="s">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="E23" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" t="s">
-        <v>63</v>
-      </c>
-      <c r="C24" t="s">
-        <v>9</v>
-      </c>
-      <c r="D24" t="s">
-        <v>32</v>
-      </c>
-      <c r="E24" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
+    <row r="25" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="B25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" t="s">
+        <v>27</v>
+      </c>
+      <c r="E25" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C26" t="s">
         <v>9</v>
       </c>
       <c r="D26" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E26" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C27" t="s">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="D27" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E27" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C28" t="s">
         <v>50</v>
       </c>
       <c r="D28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E28" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>13</v>
+        <v>140</v>
       </c>
       <c r="C29" t="s">
         <v>50</v>
       </c>
       <c r="D29" t="s">
-        <v>29</v>
+        <v>142</v>
       </c>
       <c r="E29" t="s">
-        <v>40</v>
+        <v>141</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -1448,7 +1454,7 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1475,371 +1481,371 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="D2" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="D3" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="D4" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="D5" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="D6" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="D7" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="D8" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="D9" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="D10" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="D11" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="B12" t="s">
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="D12" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B13" t="s">
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="D13" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="B14" t="s">
         <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="D14" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B15" t="s">
         <v>9</v>
       </c>
       <c r="C15" t="s">
+        <v>110</v>
+      </c>
+      <c r="D15" t="s">
         <v>118</v>
-      </c>
-      <c r="D15" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="B16" t="s">
         <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="D16" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B17" t="s">
         <v>9</v>
       </c>
       <c r="C17" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="D17" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B18" t="s">
         <v>9</v>
       </c>
       <c r="C18" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="D18" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="B19" t="s">
         <v>9</v>
       </c>
       <c r="C19" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="D19" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="B20" t="s">
         <v>9</v>
       </c>
       <c r="C20" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="D20" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="B21" t="s">
         <v>9</v>
       </c>
       <c r="C21" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="D21" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="B22" t="s">
         <v>9</v>
       </c>
       <c r="C22" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="D22" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B23" t="s">
         <v>9</v>
       </c>
       <c r="C23" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="D23" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="B24" t="s">
         <v>9</v>
       </c>
       <c r="C24" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="D24" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="B25" t="s">
         <v>9</v>
       </c>
       <c r="C25" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="D25" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="B26" t="s">
         <v>9</v>
       </c>
       <c r="C26" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="D26" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="B27" t="s">
         <v>9</v>
       </c>
       <c r="C27" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="D27" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="B28" t="s">
         <v>51</v>
@@ -1848,7 +1854,7 @@
         <v>53</v>
       </c>
       <c r="D28" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Coeff of Var input data
</commit_message>
<xml_diff>
--- a/README.xlsx
+++ b/README.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pamelagreen/Desktop/Data/Griffith2022/scripts_swb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35929780-1604-6E4A-9917-06B77519A080}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D51CF273-54B4-7B49-A64E-98E3F56B88E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41400" yWindow="-160" windowWidth="30840" windowHeight="16680" xr2:uid="{AC79CE72-321E-844F-A989-0FF187B9C603}"/>
+    <workbookView xWindow="39340" yWindow="540" windowWidth="30840" windowHeight="16680" xr2:uid="{AC79CE72-321E-844F-A989-0FF187B9C603}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="151">
   <si>
     <r>
       <rPr>
@@ -587,6 +587,30 @@
   </si>
   <si>
     <t>Vector Coast outline</t>
+  </si>
+  <si>
+    <t>CV-CDF</t>
+  </si>
+  <si>
+    <t>WBM_TerraClimate2000-2020_Q_DIST_CV_InterAnnual_6min</t>
+  </si>
+  <si>
+    <t>WBM_TerraClimate2000-2020_Q_DIST_CV_IntraAnnual_6min</t>
+  </si>
+  <si>
+    <t>WBM_TerraClimate2000-2020_Q_DIST_meanCV_IntraAnnual_6min</t>
+  </si>
+  <si>
+    <t>unitless</t>
+  </si>
+  <si>
+    <t>Inter-annual Coefficient of Variation for annual discharges across years 2000-2020</t>
+  </si>
+  <si>
+    <t>Intra-annual Coefficient of Variation of discharges across all months and years from 2000-2020</t>
+  </si>
+  <si>
+    <t>Intra-annual Coefficient of Variation across long-term mean monthly discharges for years 2000-2020</t>
   </si>
 </sst>
 </file>
@@ -1069,7 +1093,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0458106B-385E-2D4D-BF8D-F8C090212C36}">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1079,7 +1103,7 @@
     <col min="2" max="2" width="61.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
     <col min="4" max="4" width="53.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="61.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="87.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -1101,97 +1125,86 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="B3" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
       <c r="C3" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>135</v>
+        <v>147</v>
       </c>
       <c r="E3" t="s">
-        <v>136</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="C4" t="s">
-        <v>50</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
       <c r="E4" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="B6" t="s">
-        <v>68</v>
-      </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E6" t="s">
-        <v>74</v>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>146</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>147</v>
+      </c>
+      <c r="E5" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
+        <v>133</v>
+      </c>
       <c r="B7" t="s">
-        <v>69</v>
+        <v>134</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>135</v>
       </c>
       <c r="E7" t="s">
-        <v>75</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>70</v>
+        <v>137</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="D8" t="s">
-        <v>47</v>
+        <v>138</v>
       </c>
       <c r="E8" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
-        <v>71</v>
-      </c>
-      <c r="C9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" t="s">
-        <v>77</v>
+        <v>139</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="7" t="s">
+        <v>66</v>
+      </c>
       <c r="B10" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C10" t="s">
         <v>9</v>
@@ -1200,245 +1213,301 @@
         <v>47</v>
       </c>
       <c r="E10" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>57</v>
-      </c>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>22</v>
+        <v>70</v>
       </c>
       <c r="C12" t="s">
         <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="E12" t="s">
-        <v>34</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="C13" t="s">
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="E13" t="s">
-        <v>35</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
         <v>58</v>
       </c>
-      <c r="C14" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="C18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" t="s">
         <v>59</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E18" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
         <v>17</v>
       </c>
-      <c r="C15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="C19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" t="s">
         <v>60</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E19" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="7" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B21" t="s">
         <v>18</v>
       </c>
-      <c r="C17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="C21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" t="s">
         <v>33</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E21" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="7"/>
-      <c r="B18" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="7"/>
+      <c r="B22" t="s">
         <v>19</v>
       </c>
-      <c r="C18" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="C22" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" t="s">
         <v>33</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E22" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="7"/>
-      <c r="B19" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="7"/>
+      <c r="B23" t="s">
         <v>20</v>
       </c>
-      <c r="C19" t="s">
-        <v>9</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="C23" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" t="s">
         <v>33</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E23" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B20" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
         <v>21</v>
       </c>
-      <c r="C20" t="s">
-        <v>9</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="C24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" t="s">
         <v>33</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E24" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+    <row r="26" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B26" t="s">
         <v>62</v>
       </c>
-      <c r="C22" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="C26" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" t="s">
         <v>64</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E26" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" t="s">
+    <row r="27" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A27" s="4"/>
+      <c r="B27" t="s">
         <v>63</v>
       </c>
-      <c r="C23" t="s">
-        <v>9</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="C27" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" t="s">
         <v>32</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E27" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
+    <row r="29" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B29" t="s">
         <v>14</v>
       </c>
-      <c r="C25" t="s">
-        <v>9</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="C29" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29" t="s">
         <v>27</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E29" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B26" t="s">
-        <v>15</v>
-      </c>
-      <c r="C26" t="s">
-        <v>9</v>
-      </c>
-      <c r="D26" t="s">
-        <v>28</v>
-      </c>
-      <c r="E26" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B27" t="s">
-        <v>12</v>
-      </c>
-      <c r="C27" t="s">
-        <v>50</v>
-      </c>
-      <c r="D27" t="s">
-        <v>30</v>
-      </c>
-      <c r="E27" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B28" t="s">
-        <v>13</v>
-      </c>
-      <c r="C28" t="s">
-        <v>50</v>
-      </c>
-      <c r="D28" t="s">
-        <v>29</v>
-      </c>
-      <c r="E28" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B29" t="s">
-        <v>140</v>
-      </c>
-      <c r="C29" t="s">
-        <v>50</v>
-      </c>
-      <c r="D29" t="s">
-        <v>142</v>
-      </c>
-      <c r="E29" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30" t="s">
+        <v>28</v>
+      </c>
+      <c r="E30" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" t="s">
+        <v>50</v>
+      </c>
+      <c r="D31" t="s">
+        <v>30</v>
+      </c>
+      <c r="E31" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D32" t="s">
+        <v>29</v>
+      </c>
+      <c r="E32" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>140</v>
+      </c>
+      <c r="C33" t="s">
+        <v>50</v>
+      </c>
+      <c r="D33" t="s">
+        <v>142</v>
+      </c>
+      <c r="E33" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
         <v>16</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C34" t="s">
         <v>51</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D34" t="s">
         <v>31</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E34" t="s">
         <v>41</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add continent designation to README.xlsx file
</commit_message>
<xml_diff>
--- a/README.xlsx
+++ b/README.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pamelagreen/Desktop/Data/Griffith2022/scripts_swb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D51CF273-54B4-7B49-A64E-98E3F56B88E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{998774D3-1286-4243-B782-D419598355D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="39340" yWindow="540" windowWidth="30840" windowHeight="16680" xr2:uid="{AC79CE72-321E-844F-A989-0FF187B9C603}"/>
   </bookViews>
@@ -243,9 +243,6 @@
     <t>RGIS subbasin discharge point at river confluence</t>
   </si>
   <si>
-    <t>Look up table for known Basin names</t>
-  </si>
-  <si>
     <t>Annual long term Disturbed discharge from 2000-2020</t>
   </si>
   <si>
@@ -611,6 +608,9 @@
   </si>
   <si>
     <t>Intra-annual Coefficient of Variation across long-term mean monthly discharges for years 2000-2020</t>
+  </si>
+  <si>
+    <t>Look up table for known Basin names and Continent designations</t>
   </si>
 </sst>
 </file>
@@ -1028,12 +1028,12 @@
   <sheetData>
     <row r="1" spans="1:1" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
@@ -1078,12 +1078,12 @@
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1095,7 +1095,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0458106B-385E-2D4D-BF8D-F8C090212C36}">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1111,10 +1113,10 @@
         <v>8</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>48</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>49</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>24</v>
@@ -1125,100 +1127,100 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="B3" t="s">
         <v>143</v>
       </c>
-      <c r="B3" t="s">
-        <v>144</v>
-      </c>
       <c r="C3" t="s">
         <v>9</v>
       </c>
       <c r="D3" t="s">
+        <v>146</v>
+      </c>
+      <c r="E3" t="s">
         <v>147</v>
-      </c>
-      <c r="E3" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
+        <v>145</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
         <v>146</v>
       </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" t="s">
-        <v>147</v>
-      </c>
       <c r="E5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="B7" t="s">
         <v>133</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" t="s">
         <v>134</v>
       </c>
-      <c r="C7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>135</v>
-      </c>
-      <c r="E7" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
+        <v>136</v>
+      </c>
+      <c r="C8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" t="s">
         <v>137</v>
       </c>
-      <c r="C8" t="s">
-        <v>50</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>138</v>
-      </c>
-      <c r="E8" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C10" t="s">
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C11" t="s">
         <v>9</v>
@@ -1227,26 +1229,26 @@
         <v>33</v>
       </c>
       <c r="E11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C12" t="s">
         <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C13" t="s">
         <v>9</v>
@@ -1255,26 +1257,26 @@
         <v>33</v>
       </c>
       <c r="E13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C14" t="s">
         <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B16" t="s">
         <v>22</v>
@@ -1305,16 +1307,16 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" t="s">
         <v>58</v>
       </c>
-      <c r="C18" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18" t="s">
-        <v>59</v>
-      </c>
       <c r="E18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -1325,15 +1327,15 @@
         <v>9</v>
       </c>
       <c r="D19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B21" t="s">
         <v>18</v>
@@ -1345,7 +1347,7 @@
         <v>33</v>
       </c>
       <c r="E21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -1360,7 +1362,7 @@
         <v>33</v>
       </c>
       <c r="E22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -1375,7 +1377,7 @@
         <v>33</v>
       </c>
       <c r="E23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -1389,7 +1391,7 @@
         <v>33</v>
       </c>
       <c r="E24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="19" x14ac:dyDescent="0.25">
@@ -1397,22 +1399,22 @@
         <v>10</v>
       </c>
       <c r="B26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C26" t="s">
         <v>9</v>
       </c>
       <c r="D26" t="s">
+        <v>63</v>
+      </c>
+      <c r="E26" t="s">
         <v>64</v>
-      </c>
-      <c r="E26" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C27" t="s">
         <v>9</v>
@@ -1460,7 +1462,7 @@
         <v>12</v>
       </c>
       <c r="C31" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D31" t="s">
         <v>30</v>
@@ -1474,7 +1476,7 @@
         <v>13</v>
       </c>
       <c r="C32" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D32" t="s">
         <v>29</v>
@@ -1485,16 +1487,16 @@
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
+        <v>139</v>
+      </c>
+      <c r="C33" t="s">
+        <v>49</v>
+      </c>
+      <c r="D33" t="s">
+        <v>141</v>
+      </c>
+      <c r="E33" t="s">
         <v>140</v>
-      </c>
-      <c r="C33" t="s">
-        <v>50</v>
-      </c>
-      <c r="D33" t="s">
-        <v>142</v>
-      </c>
-      <c r="E33" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.2">
@@ -1502,13 +1504,13 @@
         <v>16</v>
       </c>
       <c r="C34" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D34" t="s">
         <v>31</v>
       </c>
       <c r="E34" t="s">
-        <v>41</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -1532,10 +1534,10 @@
   <sheetData>
     <row r="1" spans="1:4" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>24</v>
@@ -1546,380 +1548,380 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
       </c>
       <c r="C2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D2" t="s">
         <v>110</v>
-      </c>
-      <c r="D2" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B12" t="s">
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B13" t="s">
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B14" t="s">
         <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B15" t="s">
         <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B16" t="s">
         <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B17" t="s">
         <v>9</v>
       </c>
       <c r="C17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D17" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B18" t="s">
         <v>9</v>
       </c>
       <c r="C18" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D18" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B19" t="s">
         <v>9</v>
       </c>
       <c r="C19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B20" t="s">
         <v>9</v>
       </c>
       <c r="C20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D20" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B21" t="s">
         <v>9</v>
       </c>
       <c r="C21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D21" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B22" t="s">
         <v>9</v>
       </c>
       <c r="C22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D22" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B23" t="s">
         <v>9</v>
       </c>
       <c r="C23" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D23" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B24" t="s">
         <v>9</v>
       </c>
       <c r="C24" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B25" t="s">
         <v>9</v>
       </c>
       <c r="C25" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D25" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B26" t="s">
         <v>9</v>
       </c>
       <c r="C26" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D26" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B27" t="s">
         <v>9</v>
       </c>
       <c r="C27" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D27" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D28" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>